<commit_message>
started using Excel tables for data
</commit_message>
<xml_diff>
--- a/Grocery-Data.xlsx
+++ b/Grocery-Data.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connerhoelzle/Projects/Grocery-Price-Tracker-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0699A80-D198-BF4F-9A04-5BE3B5B7F758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920B3118-7C6A-744F-902E-B4974CAD0563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="store" sheetId="1" r:id="rId1"/>
     <sheet name="product" sheetId="2" r:id="rId2"/>
     <sheet name="receipt" sheetId="3" r:id="rId3"/>
-    <sheet name="web_session" sheetId="5" r:id="rId4"/>
-    <sheet name="line_item" sheetId="4" r:id="rId5"/>
+    <sheet name="web_session" sheetId="4" r:id="rId4"/>
+    <sheet name="line_item" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -93,6 +90,9 @@
     <t>Oak Lawn</t>
   </si>
   <si>
+    <t>Dallas Supercenter (Retail Rd)</t>
+  </si>
+  <si>
     <t>brand</t>
   </si>
   <si>
@@ -327,6 +327,96 @@
     <t>Pur</t>
   </si>
   <si>
+    <t>Sanderson Farms</t>
+  </si>
+  <si>
+    <t>Antibiotic Free Boneless Skinless Chicken Breasts</t>
+  </si>
+  <si>
+    <t>Perdue</t>
+  </si>
+  <si>
+    <t>Bluberry Bagels</t>
+  </si>
+  <si>
+    <t>L'Oven Fresh</t>
+  </si>
+  <si>
+    <t>Lender's</t>
+  </si>
+  <si>
+    <t>Three Cheese Tortellini</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Bounty Mega Roll</t>
+  </si>
+  <si>
+    <t>Bounty</t>
+  </si>
+  <si>
+    <t>Rice-a-Roni Creamy Four Cheese</t>
+  </si>
+  <si>
+    <t>Rice-a-Roni</t>
+  </si>
+  <si>
+    <t>Sesame Seed Oil</t>
+  </si>
+  <si>
+    <t>Imperial Dragon</t>
+  </si>
+  <si>
+    <t>Kewpie Mayonnaise</t>
+  </si>
+  <si>
+    <t>Kewpie</t>
+  </si>
+  <si>
+    <t>Skim Milk</t>
+  </si>
+  <si>
+    <t>Hiland</t>
+  </si>
+  <si>
+    <t>Reduced Calorie Sugar Free Syrup</t>
+  </si>
+  <si>
+    <t>Chocalate Chip Frozen Waffles</t>
+  </si>
+  <si>
+    <t>Eggo</t>
+  </si>
+  <si>
+    <t>Chicken Broth</t>
+  </si>
+  <si>
+    <t>Canned Diced Green Chilis</t>
+  </si>
+  <si>
+    <t>Black Beans</t>
+  </si>
+  <si>
+    <t>Chunky Salsa Mild</t>
+  </si>
+  <si>
+    <t>Corn Starch</t>
+  </si>
+  <si>
+    <t>Ginger Paste</t>
+  </si>
+  <si>
+    <t>Gourmet Garden</t>
+  </si>
+  <si>
+    <t>Mini Cucumbers</t>
+  </si>
+  <si>
+    <t>Produce</t>
+  </si>
+  <si>
     <t>store_id</t>
   </si>
   <si>
@@ -384,12 +474,33 @@
     <t>2025-07-17T10:33:00</t>
   </si>
   <si>
+    <t>2025-10-02T14:41:10</t>
+  </si>
+  <si>
+    <t>2025-08-03T17:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-07T19:33:26</t>
+  </si>
+  <si>
+    <t>2025-10-01T21:08:00</t>
+  </si>
+  <si>
     <t>session_date</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
+    <t>2025-09-02T09:00:00</t>
+  </si>
+  <si>
+    <t>2025-09-02T09:18:00</t>
+  </si>
+  <si>
+    <t>2025-09-02T09:21:00</t>
+  </si>
+  <si>
     <t>receipt_id</t>
   </si>
   <si>
@@ -576,84 +687,33 @@
     <t>PUR</t>
   </si>
   <si>
-    <t>2025-09-02T09:00:00</t>
-  </si>
-  <si>
-    <t>Dallas Supercenter (Retail Rd)</t>
-  </si>
-  <si>
     <t>Fresh Banana</t>
   </si>
   <si>
-    <t>Sanderson Farms</t>
-  </si>
-  <si>
     <t>Sanderson Farms Boneless Skinless Chicken Breast Fillets, 25g Protein, 4oz 112g, 1.6 - 3.05lb</t>
   </si>
   <si>
     <t>Great Value Natural Brown Long Grain Rice, 5lb (80oz)</t>
   </si>
   <si>
-    <t>2025-09-02T09:18:00</t>
-  </si>
-  <si>
-    <t>2025-09-02T09:21:00</t>
-  </si>
-  <si>
     <t>Bananas, per  lb</t>
   </si>
   <si>
-    <t>Antibiotic Free Boneless Skinless Chicken Breasts</t>
-  </si>
-  <si>
-    <t>Perdue</t>
-  </si>
-  <si>
     <t>Antibiotic Free Boneless Skinless Chicken Breasts, per  lb</t>
   </si>
   <si>
-    <t>Bluberry Bagels</t>
-  </si>
-  <si>
-    <t>L'Oven Fresh</t>
-  </si>
-  <si>
     <t>Blueberry Bagels, 20 oz</t>
   </si>
   <si>
-    <t>Lender's</t>
-  </si>
-  <si>
     <t>Lenders Original Blueberry Bagels, 6 count, Pre-sliced Refrigerated Bagels, 17.1 oz Bag</t>
   </si>
   <si>
-    <t>2025-10-02T14:41:10</t>
-  </si>
-  <si>
-    <t>Three Cheese Tortellini</t>
-  </si>
-  <si>
     <t>BAR CH TORT</t>
   </si>
   <si>
-    <t>2025-08-03T17:00:00</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
     <t>THOMAS</t>
   </si>
   <si>
-    <t>2025-08-07T19:33:26</t>
-  </si>
-  <si>
-    <t>Bounty Mega Roll</t>
-  </si>
-  <si>
-    <t>Bounty</t>
-  </si>
-  <si>
     <t>BOUNTY 1MR</t>
   </si>
   <si>
@@ -663,70 +723,7 @@
     <t>CHARMIN 6M</t>
   </si>
   <si>
-    <t>Rice-a-Roni</t>
-  </si>
-  <si>
-    <t>Rice-a-Roni Creamy Four Cheese</t>
-  </si>
-  <si>
     <t>RAR 4 CHEESE</t>
-  </si>
-  <si>
-    <t>2025-10-01T21:08:00</t>
-  </si>
-  <si>
-    <t>Sesame Seed Oil</t>
-  </si>
-  <si>
-    <t>Imperial Dragon</t>
-  </si>
-  <si>
-    <t>Kewpie Mayonnaise</t>
-  </si>
-  <si>
-    <t>Kewpie</t>
-  </si>
-  <si>
-    <t>Skim Milk</t>
-  </si>
-  <si>
-    <t>Hiland</t>
-  </si>
-  <si>
-    <t>Reduced Calorie Sugar Free Syrup</t>
-  </si>
-  <si>
-    <t>Chocalate Chip Frozen Waffles</t>
-  </si>
-  <si>
-    <t>Eggo</t>
-  </si>
-  <si>
-    <t>Chicken Broth</t>
-  </si>
-  <si>
-    <t>Canned Diced Green Chilis</t>
-  </si>
-  <si>
-    <t>Black Beans</t>
-  </si>
-  <si>
-    <t>Chunky Salsa Mild</t>
-  </si>
-  <si>
-    <t>Corn Starch</t>
-  </si>
-  <si>
-    <t>Ginger Paste</t>
-  </si>
-  <si>
-    <t>Gourmet Garden</t>
-  </si>
-  <si>
-    <t>Mini Cucumbers</t>
-  </si>
-  <si>
-    <t>Produce</t>
   </si>
   <si>
     <t>Imperial Dragon 100% Pure Sesame Seed Oil</t>
@@ -769,7 +766,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,12 +778,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -820,7 +811,23 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -831,6 +838,78 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F11E67E7-4AAE-F14D-8BBD-EA5EC100DD9E}" name="store" displayName="store" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{F11E67E7-4AAE-F14D-8BBD-EA5EC100DD9E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{83454C8C-12D6-584B-A784-F8F9059CD7C7}" name="index"/>
+    <tableColumn id="2" xr3:uid="{E65CC8D8-78E9-9348-A969-681AA6CB93D6}" name="name"/>
+    <tableColumn id="3" xr3:uid="{7ABAE3B0-CEFF-7B4B-BF55-1C2B1AD4531E}" name="location"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{199CB408-F377-264F-AF36-EB8A48E036C6}" name="product" displayName="product" ref="A1:E69" totalsRowShown="0">
+  <autoFilter ref="A1:E69" xr:uid="{199CB408-F377-264F-AF36-EB8A48E036C6}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2D525B60-F8EC-1947-A70A-5A0432695BC6}" name="index"/>
+    <tableColumn id="2" xr3:uid="{7276D8B2-58E1-6F4E-807E-18249E148D1C}" name="name"/>
+    <tableColumn id="3" xr3:uid="{08C20EE5-BF40-4F45-9638-1A0A6B5FF3FE}" name="brand"/>
+    <tableColumn id="4" xr3:uid="{09FCCEAE-7702-8F4E-AF70-90E30AE5AE2B}" name="size" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{85203C59-257A-964B-BB90-E6466379E2F1}" name="unit"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F06E788-67FC-A747-9022-DB56DACF2506}" name="receipt" displayName="receipt" ref="A1:F19" totalsRowShown="0">
+  <autoFilter ref="A1:F19" xr:uid="{6F06E788-67FC-A747-9022-DB56DACF2506}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{48FE3CE8-F17F-6F40-B05E-793C1C7839C4}" name="index"/>
+    <tableColumn id="2" xr3:uid="{10988FC4-72B6-504F-BEF4-EF060F95088D}" name="store_id"/>
+    <tableColumn id="3" xr3:uid="{EE20B898-D543-9344-A672-928A5CF1D039}" name="date"/>
+    <tableColumn id="4" xr3:uid="{DCF6761A-DB42-1E47-9A20-155DD1126BB9}" name="subtotal"/>
+    <tableColumn id="5" xr3:uid="{81E03D45-ECE2-E940-AA1B-E91D671F7145}" name="tax" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{FEDF7855-C580-8D4C-97D0-6AB9DD79AD87}" name="total_price" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A2C6AC8-EC7F-7849-92C8-E1BACB7A84B0}" name="web_session" displayName="web_session" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{2A2C6AC8-EC7F-7849-92C8-E1BACB7A84B0}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E59A0EF9-32AE-774A-90DE-CD96115B6700}" name="index"/>
+    <tableColumn id="2" xr3:uid="{F9CA26B6-D5B8-0847-B0F6-BA6630C8EBEC}" name="session_date"/>
+    <tableColumn id="3" xr3:uid="{B70DF4F0-5032-AB46-9EC1-77781B2F821E}" name="store_id"/>
+    <tableColumn id="4" xr3:uid="{3B9CB1E4-7331-7143-B3C4-8E237FDE0B7A}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CB6EC53-10A0-314F-9800-2648645776EA}" name="line_item" displayName="line_item" ref="A1:I86" totalsRowShown="0">
+  <autoFilter ref="A1:I86" xr:uid="{0CB6EC53-10A0-314F-9800-2648645776EA}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{1939EF16-56E0-764D-904B-2DEA956CFCAE}" name="index"/>
+    <tableColumn id="2" xr3:uid="{6F488941-9E84-2941-827B-6199879FB4C1}" name="receipt_id"/>
+    <tableColumn id="3" xr3:uid="{585D229C-04F9-7546-9499-C62468400D27}" name="web_session_id"/>
+    <tableColumn id="4" xr3:uid="{140AAACC-3D1B-A140-8F50-BFBE97337289}" name="product_id"/>
+    <tableColumn id="5" xr3:uid="{DFFB11CE-0429-0F45-B2B7-417B224A5B34}" name="raw_text"/>
+    <tableColumn id="6" xr3:uid="{DAC0205D-61A5-4849-BBCF-BB959774F8E4}" name="quantity"/>
+    <tableColumn id="7" xr3:uid="{262FEC05-466D-2B49-8019-FE476C9ED36B}" name="unit_price" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{09F5D0F2-2C90-B349-BD68-228580A07CC5}" name="total_price" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{CF83F4C1-8859-9B45-A916-7942A2321D44}" name="tax_status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1154,7 +1233,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1259,28 +1338,31 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073193D2-FFD8-4805-84FD-E75CF164A7EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomLeft" sqref="A1:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1291,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1305,16 +1387,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1322,16 +1404,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1339,16 +1421,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1356,16 +1438,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1373,16 +1455,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1390,16 +1472,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1407,16 +1489,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1424,16 +1506,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1441,7 +1523,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1450,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1458,16 +1540,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1475,16 +1557,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1">
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1492,16 +1574,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1509,16 +1591,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1">
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1526,16 +1608,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1">
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1543,16 +1625,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1">
         <v>14.5</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1560,16 +1642,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1577,16 +1659,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1594,16 +1676,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" s="1">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1611,16 +1693,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1628,16 +1710,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1645,16 +1727,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1662,16 +1744,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1679,16 +1761,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1696,16 +1778,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1713,16 +1795,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1730,16 +1812,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1">
         <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1747,7 +1829,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -1756,7 +1838,7 @@
         <v>25.4</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1764,16 +1846,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D29" s="1">
         <v>42</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1781,16 +1863,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D30" s="1">
         <v>450</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1798,16 +1880,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D31" s="1">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1815,16 +1897,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1">
         <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1832,16 +1914,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D33" s="1">
         <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1849,16 +1931,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34" s="1">
         <v>8.4</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1866,16 +1948,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D35" s="1">
         <v>12.5</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1883,33 +1965,33 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D36" s="1">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D37" s="1">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1917,16 +1999,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1934,16 +2016,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D39" s="1">
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1951,16 +2033,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1968,16 +2050,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D41" s="1">
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1985,16 +2067,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2002,16 +2084,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D43" s="1">
         <v>48</v>
       </c>
       <c r="E43" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2019,16 +2101,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2036,16 +2118,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2053,16 +2135,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D46" s="1">
         <v>28</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2070,16 +2152,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2087,16 +2169,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D48" s="1">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2104,16 +2186,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2121,16 +2203,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2138,16 +2220,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2155,16 +2237,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>191</v>
+        <v>100</v>
       </c>
       <c r="D52" s="1">
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2172,16 +2254,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>193</v>
+        <v>101</v>
       </c>
       <c r="D53" s="1">
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2189,16 +2271,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>196</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D54" s="1">
         <v>12</v>
       </c>
       <c r="E54" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2206,16 +2288,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="D55" s="1">
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2223,16 +2305,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
-        <v>203</v>
+        <v>105</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2240,16 +2322,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>207</v>
+        <v>107</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2257,16 +2339,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="C58" t="s">
-        <v>212</v>
+        <v>109</v>
       </c>
       <c r="D58" s="1">
         <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2274,16 +2356,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>213</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
-        <v>214</v>
+        <v>111</v>
       </c>
       <c r="D59" s="1">
         <v>15.72</v>
       </c>
       <c r="E59" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2291,16 +2373,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>216</v>
+        <v>113</v>
       </c>
       <c r="D60" s="1">
         <v>0.5</v>
       </c>
       <c r="E60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2308,16 +2390,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>217</v>
+        <v>114</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D61" s="1">
         <v>24</v>
       </c>
       <c r="E61" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2325,16 +2407,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>218</v>
+        <v>115</v>
       </c>
       <c r="C62" t="s">
-        <v>219</v>
+        <v>116</v>
       </c>
       <c r="D62" s="1">
         <v>10</v>
       </c>
       <c r="E62" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2342,16 +2424,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D63" s="1">
         <v>32</v>
       </c>
       <c r="E63" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2359,16 +2441,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>221</v>
+        <v>118</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D64" s="1">
         <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2376,16 +2458,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>222</v>
+        <v>119</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D65" s="1">
         <v>15</v>
       </c>
       <c r="E65" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2393,16 +2475,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>223</v>
+        <v>120</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D66" s="1">
         <v>16</v>
       </c>
       <c r="E66" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2410,16 +2492,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>224</v>
+        <v>121</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D67" s="1">
         <v>16</v>
       </c>
       <c r="E67" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2427,16 +2509,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>225</v>
+        <v>122</v>
       </c>
       <c r="C68" t="s">
-        <v>226</v>
+        <v>123</v>
       </c>
       <c r="D68" s="1">
         <v>4</v>
       </c>
       <c r="E68" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2444,37 +2526,42 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>228</v>
+        <v>125</v>
       </c>
       <c r="D69" s="1">
         <v>16</v>
       </c>
       <c r="E69" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D91E3C-EF95-4281-837D-622C119BD8FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="1"/>
-    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2482,19 +2569,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2505,7 +2592,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="D2">
         <v>15.99</v>
@@ -2525,7 +2612,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="D3">
         <v>100.34</v>
@@ -2545,7 +2632,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="D4">
         <v>2.2400000000000002</v>
@@ -2565,7 +2652,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="D5">
         <v>19.32</v>
@@ -2585,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="D6">
         <v>20.98</v>
@@ -2605,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="D7">
         <v>42.9</v>
@@ -2625,7 +2712,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="D8">
         <v>12.99</v>
@@ -2645,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="D9">
         <v>84.38</v>
@@ -2665,7 +2752,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="D10">
         <v>179.71</v>
@@ -2685,7 +2772,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="D11">
         <v>49.17</v>
@@ -2705,7 +2792,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="D12">
         <v>13.99</v>
@@ -2725,7 +2812,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D13">
         <v>7.33</v>
@@ -2745,7 +2832,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="D14">
         <v>3.34</v>
@@ -2765,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D15">
         <v>18.38</v>
@@ -2785,7 +2872,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="D16">
         <v>4.9800000000000004</v>
@@ -2805,7 +2892,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="D17">
         <v>3.99</v>
@@ -2825,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
       <c r="D18">
         <v>23.33</v>
@@ -2845,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>210</v>
+        <v>148</v>
       </c>
       <c r="D19">
         <v>42.12</v>
@@ -2859,16 +2946,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E46394-6DA8-4AC2-9EC2-ADED34999DFF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2883,13 +2973,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2897,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2908,7 +2998,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -2919,66 +3009,69 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B8694E-86E5-4262-9803-676FEFC78829}">
-  <dimension ref="A1:I86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="I1" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2992,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3001,11 +3094,11 @@
         <v>20</v>
       </c>
       <c r="H2" s="1">
-        <f>F2*G2</f>
+        <f t="shared" ref="H2:H33" si="0">F2*G2</f>
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3019,7 +3112,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3028,11 +3121,11 @@
         <v>20</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H66" si="0">F3*G3</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -3046,7 +3139,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -3059,7 +3152,7 @@
         <v>0.99</v>
       </c>
       <c r="I4" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3073,7 +3166,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3086,7 +3179,7 @@
         <v>12.99</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -3100,7 +3193,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3113,7 +3206,7 @@
         <v>7.99</v>
       </c>
       <c r="I6" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3124,7 +3217,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3137,7 +3230,7 @@
         <v>21.99</v>
       </c>
       <c r="I7" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3148,7 +3241,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -3161,7 +3254,7 @@
         <v>8.69</v>
       </c>
       <c r="I8" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3172,7 +3265,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3185,7 +3278,7 @@
         <v>2.69</v>
       </c>
       <c r="I9" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3196,7 +3289,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3209,7 +3302,7 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3223,7 +3316,7 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3236,7 +3329,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="I11" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3247,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -3260,7 +3353,7 @@
         <v>15.99</v>
       </c>
       <c r="I12" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3274,7 +3367,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -3287,7 +3380,7 @@
         <v>2.79</v>
       </c>
       <c r="I13" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3301,7 +3394,7 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -3314,7 +3407,7 @@
         <v>1.69</v>
       </c>
       <c r="I14" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -3328,7 +3421,7 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -3341,7 +3434,7 @@
         <v>6.99</v>
       </c>
       <c r="I15" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3355,7 +3448,7 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -3368,7 +3461,7 @@
         <v>1.35</v>
       </c>
       <c r="I16" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -3382,7 +3475,7 @@
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -3395,7 +3488,7 @@
         <v>3.95</v>
       </c>
       <c r="I17" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -3409,7 +3502,7 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -3422,7 +3515,7 @@
         <v>2.56</v>
       </c>
       <c r="I18" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -3436,7 +3529,7 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -3449,7 +3542,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="I19" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -3463,7 +3556,7 @@
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -3476,7 +3569,7 @@
         <v>8.9700000000000006</v>
       </c>
       <c r="I20" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -3490,7 +3583,7 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -3503,7 +3596,7 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -3517,7 +3610,7 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -3530,7 +3623,7 @@
         <v>2.13</v>
       </c>
       <c r="I22" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -3544,7 +3637,7 @@
         <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -3557,7 +3650,7 @@
         <v>3.72</v>
       </c>
       <c r="I23" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -3571,7 +3664,7 @@
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -3584,7 +3677,7 @@
         <v>2.97</v>
       </c>
       <c r="I24" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -3598,7 +3691,7 @@
         <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -3611,7 +3704,7 @@
         <v>0.5</v>
       </c>
       <c r="I25" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -3625,7 +3718,7 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="F26">
         <v>2.06</v>
@@ -3638,7 +3731,7 @@
         <v>1.1124000000000001</v>
       </c>
       <c r="I26" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -3652,7 +3745,7 @@
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -3665,7 +3758,7 @@
         <v>2.84</v>
       </c>
       <c r="I27" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -3679,7 +3772,7 @@
         <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -3692,7 +3785,7 @@
         <v>1.92</v>
       </c>
       <c r="I28" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -3706,7 +3799,7 @@
         <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -3719,7 +3812,7 @@
         <v>12.99</v>
       </c>
       <c r="I29" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -3733,7 +3826,7 @@
         <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -3746,7 +3839,7 @@
         <v>4.12</v>
       </c>
       <c r="I30" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -3760,7 +3853,7 @@
         <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>159</v>
+        <v>197</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -3773,7 +3866,7 @@
         <v>14.88</v>
       </c>
       <c r="I31" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -3787,7 +3880,7 @@
         <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -3800,7 +3893,7 @@
         <v>1.48</v>
       </c>
       <c r="I32" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3814,7 +3907,7 @@
         <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -3827,7 +3920,7 @@
         <v>1.48</v>
       </c>
       <c r="I33" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3841,7 +3934,7 @@
         <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>161</v>
+        <v>199</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -3850,11 +3943,11 @@
         <v>5.97</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H34:H65" si="1">F34*G34</f>
         <v>5.97</v>
       </c>
       <c r="I34" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3868,7 +3961,7 @@
         <v>32</v>
       </c>
       <c r="E35" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -3877,11 +3970,11 @@
         <v>3.57</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.57</v>
       </c>
       <c r="I35" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3895,7 +3988,7 @@
         <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -3904,11 +3997,11 @@
         <v>3.07</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.07</v>
       </c>
       <c r="I36" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3922,7 +4015,7 @@
         <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -3931,11 +4024,11 @@
         <v>8.9700000000000006</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.9700000000000006</v>
       </c>
       <c r="I37" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3949,7 +4042,7 @@
         <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -3958,11 +4051,11 @@
         <v>3</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3976,7 +4069,7 @@
         <v>34</v>
       </c>
       <c r="E39" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -3985,11 +4078,11 @@
         <v>3</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -4003,7 +4096,7 @@
         <v>19</v>
       </c>
       <c r="E40" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -4012,11 +4105,11 @@
         <v>3.72</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.72</v>
       </c>
       <c r="I40" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -4030,7 +4123,7 @@
         <v>35</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -4039,11 +4132,11 @@
         <v>3.98</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
       <c r="I41" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -4057,7 +4150,7 @@
         <v>36</v>
       </c>
       <c r="E42" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -4066,11 +4159,11 @@
         <v>9.1199999999999992</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1199999999999992</v>
       </c>
       <c r="I42" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -4084,7 +4177,7 @@
         <v>37</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -4093,11 +4186,11 @@
         <v>3.17</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.17</v>
       </c>
       <c r="I43" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -4111,7 +4204,7 @@
         <v>38</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -4120,11 +4213,11 @@
         <v>0.98</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.98</v>
       </c>
       <c r="I44" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -4138,7 +4231,7 @@
         <v>38</v>
       </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -4147,11 +4240,11 @@
         <v>0.98</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.98</v>
       </c>
       <c r="I45" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -4165,7 +4258,7 @@
         <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="F46">
         <v>2.78</v>
@@ -4174,11 +4267,11 @@
         <v>0.54</v>
       </c>
       <c r="H46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5012000000000001</v>
       </c>
       <c r="I46" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -4192,7 +4285,7 @@
         <v>40</v>
       </c>
       <c r="E47" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4201,11 +4294,11 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="I47" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4219,7 +4312,7 @@
         <v>41</v>
       </c>
       <c r="E48" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="F48">
         <v>2.12</v>
@@ -4228,14 +4321,14 @@
         <v>1.58</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3496000000000001</v>
       </c>
       <c r="I48" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4246,7 +4339,7 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -4255,14 +4348,14 @@
         <v>2.69</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.38</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4273,7 +4366,7 @@
         <v>42</v>
       </c>
       <c r="E50" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="F50">
         <v>2</v>
@@ -4282,14 +4375,14 @@
         <v>5.99</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.98</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4300,7 +4393,7 @@
         <v>45</v>
       </c>
       <c r="E51" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -4309,14 +4402,14 @@
         <v>12.99</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.99</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4327,7 +4420,7 @@
         <v>46</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -4336,14 +4429,14 @@
         <v>9.19</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.38</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4354,7 +4447,7 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -4363,11 +4456,11 @@
         <v>7.99</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -4381,7 +4474,7 @@
         <v>47</v>
       </c>
       <c r="E54" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -4390,7 +4483,7 @@
         <v>13.99</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.99</v>
       </c>
     </row>
@@ -4405,7 +4498,7 @@
         <v>46</v>
       </c>
       <c r="E55" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -4414,11 +4507,11 @@
         <v>7.99</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
       <c r="I55" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -4432,7 +4525,7 @@
         <v>48</v>
       </c>
       <c r="E56" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -4441,11 +4534,11 @@
         <v>8.19</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.19</v>
       </c>
       <c r="I56" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -4459,7 +4552,7 @@
         <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -4468,7 +4561,7 @@
         <v>0.48</v>
       </c>
       <c r="H57" s="1">
-        <f>F57*G57</f>
+        <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
     </row>
@@ -4483,7 +4576,7 @@
         <v>49</v>
       </c>
       <c r="E58" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -4492,7 +4585,7 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6399999999999997</v>
       </c>
     </row>
@@ -4507,7 +4600,7 @@
         <v>35</v>
       </c>
       <c r="E59" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -4516,7 +4609,7 @@
         <v>3.98</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
     </row>
@@ -4531,7 +4624,7 @@
         <v>35</v>
       </c>
       <c r="E60" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -4540,7 +4633,7 @@
         <v>3.98</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
     </row>
@@ -4555,7 +4648,7 @@
         <v>49</v>
       </c>
       <c r="E61" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -4564,7 +4657,7 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6399999999999997</v>
       </c>
     </row>
@@ -4579,7 +4672,7 @@
         <v>22</v>
       </c>
       <c r="E62" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -4588,7 +4681,7 @@
         <v>0.5</v>
       </c>
       <c r="H62" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -4603,7 +4696,7 @@
         <v>22</v>
       </c>
       <c r="E63" t="s">
-        <v>186</v>
+        <v>219</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -4612,7 +4705,7 @@
         <v>0.48</v>
       </c>
       <c r="H63" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
     </row>
@@ -4627,7 +4720,7 @@
         <v>50</v>
       </c>
       <c r="E64" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -4636,7 +4729,7 @@
         <v>4.29</v>
       </c>
       <c r="H64" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.29</v>
       </c>
     </row>
@@ -4651,7 +4744,7 @@
         <v>51</v>
       </c>
       <c r="E65" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -4660,7 +4753,7 @@
         <v>2.19</v>
       </c>
       <c r="H65" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.19</v>
       </c>
     </row>
@@ -4675,7 +4768,7 @@
         <v>52</v>
       </c>
       <c r="E66" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -4684,7 +4777,7 @@
         <v>2.72</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H66:H69" si="2">F66*G66</f>
         <v>2.72</v>
       </c>
     </row>
@@ -4699,7 +4792,7 @@
         <v>52</v>
       </c>
       <c r="E67" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -4708,7 +4801,7 @@
         <v>2.72</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" ref="H67:H69" si="1">F67*G67</f>
+        <f t="shared" si="2"/>
         <v>2.72</v>
       </c>
     </row>
@@ -4723,7 +4816,7 @@
         <v>53</v>
       </c>
       <c r="E68" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -4732,11 +4825,11 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="H68" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9800000000000004</v>
       </c>
       <c r="I68" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -4750,7 +4843,7 @@
         <v>54</v>
       </c>
       <c r="E69" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -4759,11 +4852,11 @@
         <v>3.99</v>
       </c>
       <c r="H69" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.99</v>
       </c>
       <c r="I69" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -4777,7 +4870,7 @@
         <v>46</v>
       </c>
       <c r="E70" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="F70">
         <v>2</v>
@@ -4789,7 +4882,7 @@
         <v>18.38</v>
       </c>
       <c r="I70" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -4803,7 +4896,7 @@
         <v>55</v>
       </c>
       <c r="E71" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -4815,7 +4908,7 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="I71" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -4829,7 +4922,7 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -4841,7 +4934,7 @@
         <v>7.97</v>
       </c>
       <c r="I72" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -4855,7 +4948,7 @@
         <v>56</v>
       </c>
       <c r="E73" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -4867,7 +4960,7 @@
         <v>1.33</v>
       </c>
       <c r="I73" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -4904,7 +4997,7 @@
         <v>58</v>
       </c>
       <c r="E75" t="s">
-        <v>213</v>
+        <v>110</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -5169,12 +5262,27 @@
         <v>1.97</v>
       </c>
     </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G87"/>
+      <c r="H87"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G88"/>
+      <c r="H88"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G89"/>
+      <c r="H89"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{8F6DE934-DEF0-4304-A10D-2A369C4EC76C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"T,NF,T+,F,FA,O,N,X"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>